<commit_message>
Netherlands API is done.
</commit_message>
<xml_diff>
--- a/doc/Mapping.xlsx
+++ b/doc/Mapping.xlsx
@@ -5,14 +5,14 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stanie\git\netherlands-api\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\servaism\Documents\1-Clients\CPSV-AP\Support to Member states\Netherlands\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7650"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Mapping SRU - CPSV-AP" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -536,12 +536,6 @@
     <xf numFmtId="43" fontId="3" fillId="4" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -572,6 +566,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -876,49 +876,49 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.33203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="83.9140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.4140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.08203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="83.875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.125" style="1" customWidth="1"/>
     <col min="5" max="5" width="14.5" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="32.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.33203125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.33203125" style="1"/>
+    <col min="7" max="7" width="19.375" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-    </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+    </row>
+    <row r="2" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="25"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
       <c r="G4" s="9"/>
     </row>
-    <row r="5" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>23</v>
       </c>
@@ -941,8 +941,8 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="15" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="13" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="6" t="s">
@@ -964,8 +964,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="16" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="14" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
@@ -987,8 +987,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="16" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="14" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
@@ -997,7 +997,7 @@
       <c r="C9" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="19" t="s">
         <v>45</v>
       </c>
       <c r="E9" s="6" t="s">
@@ -1010,8 +1010,8 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="16" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="14" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
@@ -1033,31 +1033,31 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="17" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="18" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="E11" s="18" t="s">
         <v>39</v>
       </c>
       <c r="F11" t="s">
         <v>20</v>
       </c>
-      <c r="G11" s="24" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="16" t="s">
+      <c r="G11" s="22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="14" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
@@ -1072,15 +1072,15 @@
       <c r="E12" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F12" s="23" t="s">
+      <c r="F12" s="21" t="s">
         <v>35</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="16" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="14" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="6" t="s">
@@ -1089,21 +1089,21 @@
       <c r="C13" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="D13" s="20" t="s">
         <v>42</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F13" s="23" t="s">
+      <c r="F13" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="G13" s="25" t="s">
+      <c r="G13" s="23" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="16" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="14" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="6" t="s">
@@ -1118,15 +1118,15 @@
       <c r="E14" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F14" s="23" t="s">
+      <c r="F14" s="21" t="s">
         <v>20</v>
       </c>
       <c r="G14" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="16" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="14" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="6" t="s">
@@ -1141,15 +1141,15 @@
       <c r="E15" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="23" t="s">
+      <c r="F15" s="21" t="s">
         <v>20</v>
       </c>
       <c r="G15" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="16" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="14" t="s">
         <v>18</v>
       </c>
       <c r="B16" s="6" t="s">
@@ -1164,15 +1164,15 @@
       <c r="E16" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="23" t="s">
+      <c r="F16" s="21" t="s">
         <v>20</v>
       </c>
       <c r="G16" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="16" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="6" t="s">
@@ -1187,15 +1187,15 @@
       <c r="E17" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F17" s="23" t="s">
+      <c r="F17" s="21" t="s">
         <v>20</v>
       </c>
       <c r="G17" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="16" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="14" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="6" t="s">
@@ -1204,21 +1204,21 @@
       <c r="C18" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D18" s="21" t="s">
+      <c r="D18" s="19" t="s">
         <v>46</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F18" s="23" t="s">
+      <c r="F18" s="21" t="s">
         <v>21</v>
       </c>
       <c r="G18" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="16" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="14" t="s">
         <v>26</v>
       </c>
       <c r="B19" s="6" t="s">
@@ -1227,21 +1227,21 @@
       <c r="C19" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="19" t="s">
+      <c r="D19" s="17" t="s">
         <v>46</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F19" s="23" t="s">
+      <c r="F19" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G19" s="25" t="s">
+      <c r="G19" s="23" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="16" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="14" t="s">
         <v>28</v>
       </c>
       <c r="B20" s="6" t="s">
@@ -1256,15 +1256,15 @@
       <c r="E20" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F20" s="23" t="s">
+      <c r="F20" s="21" t="s">
         <v>20</v>
       </c>
       <c r="G20" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="16" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="14" t="s">
         <v>29</v>
       </c>
       <c r="B21" s="6" t="s">
@@ -1279,15 +1279,15 @@
       <c r="E21" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F21" s="23" t="s">
+      <c r="F21" s="21" t="s">
         <v>38</v>
       </c>
       <c r="G21" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="16" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="14" t="s">
         <v>30</v>
       </c>
       <c r="B22" s="6" t="s">
@@ -1309,8 +1309,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="16" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="14" t="s">
         <v>31</v>
       </c>
       <c r="B23" s="6" t="s">
@@ -1332,8 +1332,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="18" t="s">
+    <row r="24" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="16" t="s">
         <v>32</v>
       </c>
       <c r="B24" s="10" t="s">
@@ -1355,12 +1355,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>54</v>
       </c>

</xml_diff>